<commit_message>
framework stabilization and hydroflesk cases commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139F3819-BFE9-4B62-8CC1-1F7B33CDAC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12D53C4-7610-4982-A5EC-5A3492917CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>UserName</t>
   </si>
@@ -70,9 +70,6 @@
     <t>VISA</t>
   </si>
   <si>
-    <t>Jun</t>
-  </si>
-  <si>
     <t>Street</t>
   </si>
   <si>
@@ -101,6 +98,12 @@
   </si>
   <si>
     <t>cvv</t>
+  </si>
+  <si>
+    <t>4444444444444448</t>
+  </si>
+  <si>
+    <t>Feb</t>
   </si>
 </sst>
 </file>
@@ -154,12 +157,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,34 +481,34 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -546,7 +552,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -554,17 +560,17 @@
       <c r="L4" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="3">
-        <v>2345234523452340</v>
+      <c r="M4" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="N4" s="4">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="O4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="P4" s="3">
-        <v>345</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revlon US Invalid Credit card checkout test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8EDB93-1FFB-40CE-9E22-D7A68BA7E479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47667BE8-D30D-4EC4-8489-2C6495D9F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>UserName</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>Nice Product for Hair dryer</t>
+  </si>
+  <si>
+    <t>InvalidCreditCard</t>
+  </si>
+  <si>
+    <t>1212121212121212</t>
   </si>
 </sst>
 </file>
@@ -605,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,83 +829,48 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="S6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6" t="s">
-        <v>26</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>28</v>
+      <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2021</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>53</v>
+      </c>
+      <c r="R6" s="3">
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7">
-        <v>12345</v>
-      </c>
-      <c r="M7" s="3">
-        <v>9898989899</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
       <c r="S7" t="s">
         <v>29</v>
       </c>
       <c r="T7" t="s">
-        <v>46</v>
-      </c>
-      <c r="W7">
-        <v>12341</v>
-      </c>
-      <c r="X7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>5</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>2020</v>
+        <v>26</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -955,7 +926,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -967,101 +938,157 @@
         <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
         <v>40</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>64</v>
+        <v>41</v>
+      </c>
+      <c r="L9">
+        <v>12345</v>
       </c>
       <c r="M9" s="3">
         <v>9898989899</v>
       </c>
+      <c r="S9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9">
+        <v>12341</v>
+      </c>
+      <c r="X9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>2020</v>
+      </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="S10" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="3">
+        <v>9898989899</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="S11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" t="s">
-        <v>70</v>
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="S14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>74</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AB17" t="s">
         <v>29</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AC17" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1070,14 +1097,14 @@
     <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
-    <hyperlink ref="U6" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
-    <hyperlink ref="V6" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{1E5A79C9-9C18-42C3-B520-7BD394A6C354}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
+    <hyperlink ref="U7" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
+    <hyperlink ref="V7" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{1E5A79C9-9C18-42C3-B520-7BD394A6C354}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
     <hyperlink ref="B3" r:id="rId10" xr:uid="{528A7A19-561A-4E3E-A382-9CEA86404515}"/>
-    <hyperlink ref="F16" r:id="rId11" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
+    <hyperlink ref="F17" r:id="rId11" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId12"/>

</xml_diff>

<commit_message>
Code Optimization for Revlon UK, Revlon & Hottools
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47667BE8-D30D-4EC4-8489-2C6495D9F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A8CDBD-4E2D-47DB-8D01-8440899DE17C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
   <si>
     <t>UserName</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>1212121212121212</t>
+  </si>
+  <si>
+    <t>Salon One-Step Hair Dryer And Volumizer In Blue</t>
   </si>
 </sst>
 </file>
@@ -613,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +636,7 @@
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -856,7 +859,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="S7" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="T7" t="s">
         <v>26</v>
@@ -903,7 +906,7 @@
         <v>9898989899</v>
       </c>
       <c r="S8" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="T8" t="s">
         <v>46</v>
@@ -959,7 +962,7 @@
         <v>9898989899</v>
       </c>
       <c r="S9" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="T9" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Revlon US & UK Code Commit for Mobile and Web Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A8CDBD-4E2D-47DB-8D01-8440899DE17C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9942D1B7-B234-4388-B598-0DCEBAE990B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>UserName</t>
   </si>
@@ -263,6 +263,30 @@
   </si>
   <si>
     <t>Salon One-Step Hair Dryer And Volumizer In Blue</t>
+  </si>
+  <si>
+    <t>HeaderLinks</t>
+  </si>
+  <si>
+    <t>HeaderNames</t>
+  </si>
+  <si>
+    <t>Dryers,Straighteners,Curling Irons,Hair Brushes &amp; Elastics,Specialty</t>
+  </si>
+  <si>
+    <t>HeaderMobileLinks</t>
+  </si>
+  <si>
+    <t>Collections,Dryers,Straighteners,Curling Irons,Hair Brushes &amp; Elastics,Specialty</t>
+  </si>
+  <si>
+    <t>Promocode</t>
+  </si>
+  <si>
+    <t>20OFF!</t>
+  </si>
+  <si>
+    <t>1" Long Lasting Curls Heated Silicone Brush</t>
   </si>
 </sst>
 </file>
@@ -614,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,9 +669,11 @@
     <col min="26" max="27" width="9.140625" style="6"/>
     <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="70.42578125" customWidth="1"/>
+    <col min="31" max="31" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -735,8 +761,14 @@
       <c r="AC1" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -756,7 +788,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -776,7 +808,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -809,7 +841,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -830,7 +862,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -851,7 +883,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -871,7 +903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -927,7 +959,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -983,7 +1015,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -1018,7 +1050,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1026,7 +1058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1046,7 +1078,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1054,7 +1086,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1062,7 +1094,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1070,7 +1102,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1078,7 +1110,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1093,6 +1125,33 @@
       </c>
       <c r="AC17" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="S20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RevlonUS Latest Changes and Expansion
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9942D1B7-B234-4388-B598-0DCEBAE990B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66706E9E-E305-4C87-B59B-C3B36B486F61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
   <si>
     <t>UserName</t>
   </si>
@@ -287,6 +287,36 @@
   </si>
   <si>
     <t>1" Long Lasting Curls Heated Silicone Brush</t>
+  </si>
+  <si>
+    <t>PaymentDetailsDiscoverCard</t>
+  </si>
+  <si>
+    <t>Discover</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>PaymentDetailsAMEXCard</t>
+  </si>
+  <si>
+    <t>AMEX</t>
+  </si>
+  <si>
+    <t>PaymentDetailsMasterCard</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>5500005555555559</t>
+  </si>
+  <si>
+    <t>6011000995500000</t>
+  </si>
+  <si>
+    <t>371449635398431</t>
   </si>
 </sst>
 </file>
@@ -638,15 +668,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE20"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="J10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -658,7 +688,7 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1153,6 +1183,75 @@
       <c r="AE20" t="s">
         <v>87</v>
       </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="N21" t="s">
+        <v>90</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P21">
+        <v>2030</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>91</v>
+      </c>
+      <c r="R21">
+        <v>737</v>
+      </c>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="N22" t="s">
+        <v>93</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P22">
+        <v>2030</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>91</v>
+      </c>
+      <c r="R22">
+        <v>7371</v>
+      </c>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="N23" t="s">
+        <v>95</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="P23">
+        <v>2030</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R23">
+        <v>737</v>
+      </c>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Revlon US 10 Expansion Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66706E9E-E305-4C87-B59B-C3B36B486F61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A76661-0BB4-4710-9BD4-F215AF27A21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
   <si>
     <t>UserName</t>
   </si>
@@ -286,37 +286,46 @@
     <t>20OFF!</t>
   </si>
   <si>
+    <t>PaymentDetailsDiscoverCard</t>
+  </si>
+  <si>
+    <t>Discover</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>PaymentDetailsAMEXCard</t>
+  </si>
+  <si>
+    <t>AMEX</t>
+  </si>
+  <si>
+    <t>PaymentDetailsMasterCard</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>5500005555555559</t>
+  </si>
+  <si>
+    <t>6011000995500000</t>
+  </si>
+  <si>
+    <t>371449635398431</t>
+  </si>
+  <si>
+    <t>NewAddress</t>
+  </si>
+  <si>
+    <t>54 N Hermitage Ave Chicago Il 60612</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
     <t>1" Long Lasting Curls Heated Silicone Brush</t>
-  </si>
-  <si>
-    <t>PaymentDetailsDiscoverCard</t>
-  </si>
-  <si>
-    <t>Discover</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>PaymentDetailsAMEXCard</t>
-  </si>
-  <si>
-    <t>AMEX</t>
-  </si>
-  <si>
-    <t>PaymentDetailsMasterCard</t>
-  </si>
-  <si>
-    <t>MasterCard</t>
-  </si>
-  <si>
-    <t>5500005555555559</t>
-  </si>
-  <si>
-    <t>6011000995500000</t>
-  </si>
-  <si>
-    <t>371449635398431</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +357,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -377,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -387,6 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -668,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" topLeftCell="H9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,8 +856,9 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>21</v>
@@ -849,8 +866,9 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
         <v>40</v>
@@ -859,49 +877,61 @@
         <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
       <c r="L4">
-        <v>12345</v>
-      </c>
-      <c r="M4" s="3">
-        <v>9898989899</v>
+        <v>60612</v>
+      </c>
+      <c r="M4">
+        <v>9865321478</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="N5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="4">
-        <v>2021</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>53</v>
-      </c>
-      <c r="R5" s="3">
-        <v>737</v>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>12345</v>
+      </c>
+      <c r="M5" s="3">
+        <v>9898989899</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1"/>
       <c r="N6" t="s">
         <v>10</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="P6" s="4">
         <v>2021</v>
@@ -915,83 +945,48 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="S7" t="s">
-        <v>80</v>
-      </c>
-      <c r="T7" t="s">
-        <v>26</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>28</v>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="P7" s="4">
+        <v>2021</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R7" s="3">
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8">
-        <v>12345</v>
-      </c>
-      <c r="M8" s="3">
-        <v>9898989899</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
       <c r="S8" t="s">
         <v>80</v>
       </c>
       <c r="T8" t="s">
-        <v>46</v>
-      </c>
-      <c r="W8">
-        <v>12341</v>
-      </c>
-      <c r="X8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y8" s="6">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>2020</v>
+        <v>26</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -1047,7 +1042,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -1059,172 +1054,205 @@
         <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
         <v>40</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>64</v>
+        <v>41</v>
+      </c>
+      <c r="L10">
+        <v>12345</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
       </c>
+      <c r="S10" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W10">
+        <v>12341</v>
+      </c>
+      <c r="X10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>2020</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="S11" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11" s="3">
+        <v>9898989899</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="S12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="S13" t="s">
-        <v>70</v>
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="S15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+      <c r="S17" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>85</v>
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AD19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="S20" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
-      </c>
-      <c r="N21" t="s">
-        <v>90</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="P21">
-        <v>2030</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>91</v>
-      </c>
-      <c r="R21">
-        <v>737</v>
-      </c>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
+        <v>86</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P22">
         <v>2030</v>
       </c>
       <c r="Q22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R22">
-        <v>7371</v>
+        <v>737</v>
       </c>
       <c r="Y22"/>
       <c r="Z22"/>
@@ -1232,40 +1260,63 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P23">
         <v>2030</v>
       </c>
       <c r="Q23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R23">
-        <v>737</v>
+        <v>7371</v>
       </c>
       <c r="Y23"/>
       <c r="Z23"/>
       <c r="AA23"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="N24" t="s">
+        <v>94</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="P24">
+        <v>2030</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>90</v>
+      </c>
+      <c r="R24">
+        <v>737</v>
+      </c>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
-    <hyperlink ref="U7" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
-    <hyperlink ref="V7" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{1E5A79C9-9C18-42C3-B520-7BD394A6C354}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
+    <hyperlink ref="U8" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
+    <hyperlink ref="V8" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{1E5A79C9-9C18-42C3-B520-7BD394A6C354}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
     <hyperlink ref="B3" r:id="rId10" xr:uid="{528A7A19-561A-4E3E-A382-9CEA86404515}"/>
-    <hyperlink ref="F17" r:id="rId11" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
+    <hyperlink ref="F18" r:id="rId11" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId12"/>

</xml_diff>

<commit_message>
Testdata commit - RevlonUS
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC9F65-0A8C-4763-94B7-48C3A3214287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0871FA56-3F57-4123-AFDA-5361F7C4A398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -331,12 +331,6 @@
     <t>New Mexico</t>
   </si>
   <si>
-    <t>dbethi@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Divya@123</t>
-  </si>
-  <si>
     <t>Divyasri</t>
   </si>
   <si>
@@ -398,6 +392,12 @@
   </si>
   <si>
     <t>02478</t>
+  </si>
+  <si>
+    <t>skatipelli@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Saikumar@1548</t>
   </si>
 </sst>
 </file>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:M16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>16</v>
@@ -931,7 +931,7 @@
         <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
         <v>95</v>
@@ -951,7 +951,7 @@
         <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
         <v>95</v>
@@ -967,26 +967,26 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
         <v>95</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H4" t="s">
         <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J4" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="L4" s="14">
         <v>81100</v>
@@ -997,25 +997,25 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -1024,10 +1024,10 @@
         <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L5" s="15">
         <v>19702</v>
@@ -1043,14 +1043,14 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
         <v>95</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
         <v>95</v>
@@ -1086,7 +1086,7 @@
         <v>96</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -1095,7 +1095,7 @@
         <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
@@ -1119,7 +1119,7 @@
         <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
         <v>95</v>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
         <v>95</v>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
         <v>95</v>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E11" t="s">
         <v>95</v>
@@ -1247,7 +1247,7 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
         <v>95</v>
@@ -1271,7 +1271,7 @@
         <v>37</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M12" s="3">
         <v>9898989899</v>
@@ -1304,7 +1304,7 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E13" t="s">
         <v>95</v>
@@ -1328,7 +1328,7 @@
         <v>37</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M13" s="3">
         <v>9898989899</v>
@@ -1361,7 +1361,7 @@
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
         <v>95</v>
@@ -1397,7 +1397,7 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
         <v>95</v>
@@ -1417,7 +1417,7 @@
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
         <v>95</v>
@@ -1449,7 +1449,7 @@
         <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
         <v>95</v>
@@ -1463,7 +1463,7 @@
         <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
         <v>95</v>
@@ -1477,7 +1477,7 @@
         <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
         <v>95</v>
@@ -1491,7 +1491,7 @@
         <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
         <v>95</v>
@@ -1505,7 +1505,7 @@
         <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E21" t="s">
         <v>95</v>
@@ -1541,7 +1541,7 @@
         <v>79</v>
       </c>
       <c r="T24" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AF24" t="s">
         <v>80</v>
@@ -1627,36 +1627,36 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" t="s">
         <v>104</v>
       </c>
-      <c r="D28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" t="s">
-        <v>106</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1674,13 +1674,13 @@
     <hyperlink ref="B5" r:id="rId11" xr:uid="{1167FB23-6AA4-48EB-9787-A4DC54F3BA79}"/>
     <hyperlink ref="F8" r:id="rId12" xr:uid="{ED3E7E5C-CDBB-4070-A72C-5165E49FF350}"/>
     <hyperlink ref="C5" r:id="rId13" xr:uid="{1047C4BB-4BDF-4DD9-9CA0-154BCFB1A6FA}"/>
-    <hyperlink ref="F5" r:id="rId14" xr:uid="{C1B467EC-607C-4F9F-8896-0938FB5BEC03}"/>
-    <hyperlink ref="B28" r:id="rId15" xr:uid="{2F5252AC-7F34-4980-AB64-18367B62468F}"/>
-    <hyperlink ref="C28" r:id="rId16" xr:uid="{C7CD3122-A25C-43C6-9109-D0B89281977C}"/>
-    <hyperlink ref="F28" r:id="rId17" xr:uid="{4E518ECA-3986-4097-AD5C-2E2942132CF0}"/>
-    <hyperlink ref="B29" r:id="rId18" xr:uid="{DC221449-F2C2-47EA-A36C-5A7D61EB66BF}"/>
-    <hyperlink ref="C29" r:id="rId19" xr:uid="{308319C9-BDF0-4490-8182-131D9C004226}"/>
-    <hyperlink ref="F29" r:id="rId20" xr:uid="{90DE5CFD-F116-42E7-B1A7-048ED9497115}"/>
+    <hyperlink ref="B28" r:id="rId14" xr:uid="{2F5252AC-7F34-4980-AB64-18367B62468F}"/>
+    <hyperlink ref="C28" r:id="rId15" xr:uid="{C7CD3122-A25C-43C6-9109-D0B89281977C}"/>
+    <hyperlink ref="B29" r:id="rId16" xr:uid="{DC221449-F2C2-47EA-A36C-5A7D61EB66BF}"/>
+    <hyperlink ref="C29" r:id="rId17" xr:uid="{308319C9-BDF0-4490-8182-131D9C004226}"/>
+    <hyperlink ref="F29" r:id="rId18" xr:uid="{90DE5CFD-F116-42E7-B1A7-048ED9497115}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{FFE2EABE-20E2-44BD-97D7-7B5F1FD84BB6}"/>
+    <hyperlink ref="F5" r:id="rId20" xr:uid="{6E25E14F-3359-4AB4-AEFC-BF4A3F34EFE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId21"/>

</xml_diff>

<commit_message>
RevlonUS - Updated code commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBC838C-CBEB-41BC-B5AE-6F292F2BC6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="1530" windowWidth="15345" windowHeight="6270"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="152">
   <si>
     <t>UserName</t>
   </si>
@@ -399,27 +400,15 @@
     <t>Atlanta</t>
   </si>
   <si>
-    <t>GEORGIA</t>
-  </si>
-  <si>
     <t>taxrate</t>
   </si>
   <si>
-    <t>Colorado Springs</t>
-  </si>
-  <si>
-    <t>4421 Millburn Dr</t>
-  </si>
-  <si>
     <t>Volume Booster Hair Dryer</t>
   </si>
   <si>
     <t>50$belowproduct</t>
   </si>
   <si>
-    <t>Colorado</t>
-  </si>
-  <si>
     <t>712 Mill Walk NW</t>
   </si>
   <si>
@@ -456,20 +445,47 @@
     <t>sukesh123@</t>
   </si>
   <si>
-    <t>Salon One-Step Hair Dryer And Volumizer In Blue</t>
-  </si>
-  <si>
     <t>Salon One-Step Hair Dryer And VolumizerIn Blue</t>
+  </si>
+  <si>
+    <t>giftcard</t>
+  </si>
+  <si>
+    <t>012QALEJIIFB</t>
+  </si>
+  <si>
+    <t>salon one-step hair dryer and volumizer in blue</t>
+  </si>
+  <si>
+    <t>Applygiftcard</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>7.75</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Meriden</t>
+  </si>
+  <si>
+    <t>06450</t>
+  </si>
+  <si>
+    <t>6.35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -568,6 +584,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -842,21 +870,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
@@ -869,7 +897,8 @@
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="13" width="11.85546875" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="13" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="19" customWidth="1"/>
     <col min="14" max="15" width="15.85546875" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -886,9 +915,10 @@
     <col min="32" max="33" width="70.42578125" customWidth="1"/>
     <col min="34" max="34" width="16.28515625" customWidth="1"/>
     <col min="35" max="35" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -925,8 +955,8 @@
       <c r="L1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="12" t="s">
-        <v>127</v>
+      <c r="M1" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>15</v>
@@ -986,21 +1016,24 @@
         <v>74</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AH1" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
+        <v>130</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>92</v>
@@ -1012,10 +1045,10 @@
         <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1032,10 +1065,10 @@
         <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -1048,7 +1081,7 @@
         <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>115</v>
@@ -1068,17 +1101,17 @@
       <c r="L4" s="14">
         <v>81100</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="20"/>
       <c r="N4">
         <v>7856978455</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>92</v>
@@ -1090,7 +1123,7 @@
         <v>93</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>106</v>
@@ -1110,14 +1143,14 @@
       <c r="L5" s="15">
         <v>19702</v>
       </c>
-      <c r="M5" s="15">
-        <v>0</v>
+      <c r="M5" s="21" t="s">
+        <v>148</v>
       </c>
       <c r="N5">
         <v>8756941256</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="17.25" customHeight="1">
+    <row r="6" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -1130,10 +1163,10 @@
         <v>93</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -1145,19 +1178,19 @@
         <v>125</v>
       </c>
       <c r="K6" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="L6" s="15">
         <v>30327</v>
       </c>
-      <c r="M6" s="15">
-        <v>7.75</v>
+      <c r="M6" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="N6">
         <v>8756941256</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1170,10 +1203,10 @@
         <v>93</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -1182,27 +1215,27 @@
         <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="K7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L7" s="15">
-        <v>80906</v>
-      </c>
-      <c r="M7" s="15">
-        <v>2.9</v>
+        <v>57</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="N7">
         <v>8756941256</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
@@ -1212,7 +1245,7 @@
         <v>93</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G8" t="s">
         <v>103</v>
@@ -1236,7 +1269,7 @@
         <v>9865321478</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1248,7 +1281,7 @@
         <v>93</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G9" t="s">
         <v>104</v>
@@ -1273,15 +1306,15 @@
       </c>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
         <v>120</v>
@@ -1290,7 +1323,7 @@
         <v>93</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G10" t="s">
         <v>98</v>
@@ -1315,7 +1348,7 @@
       </c>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1360,7 @@
         <v>93</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
@@ -1351,7 +1384,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -1363,7 +1396,7 @@
         <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I12" t="s">
         <v>31</v>
@@ -1384,9 +1417,9 @@
         <v>737</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" t="s">
@@ -1402,13 +1435,13 @@
       <c r="R13" s="4"/>
       <c r="T13" s="3"/>
       <c r="U13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AI13" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1458,7 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="U14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V14" t="s">
         <v>22</v>
@@ -1437,10 +1470,10 @@
         <v>24</v>
       </c>
       <c r="AI14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1451,7 +1484,7 @@
         <v>93</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G15" t="s">
         <v>30</v>
@@ -1471,13 +1504,13 @@
       <c r="L15" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="M15" s="15"/>
+      <c r="M15" s="21"/>
       <c r="N15" s="3">
         <v>9898989899</v>
       </c>
       <c r="O15" s="3"/>
       <c r="U15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V15" t="s">
         <v>41</v>
@@ -1498,10 +1531,10 @@
         <v>2020</v>
       </c>
       <c r="AI15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1512,7 +1545,7 @@
         <v>93</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G16" t="s">
         <v>30</v>
@@ -1532,13 +1565,13 @@
       <c r="L16" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="M16" s="15"/>
+      <c r="M16" s="21"/>
       <c r="N16" s="3">
         <v>9898989899</v>
       </c>
       <c r="O16" s="3"/>
       <c r="U16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V16" t="s">
         <v>41</v>
@@ -1559,10 +1592,10 @@
         <v>2020</v>
       </c>
       <c r="AI16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1573,7 +1606,7 @@
         <v>93</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G17" t="s">
         <v>55</v>
@@ -1593,13 +1626,13 @@
       <c r="L17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="21"/>
       <c r="N17" s="3">
         <v>9898989899</v>
       </c>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1610,13 +1643,13 @@
         <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="U18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1633,7 +1666,7 @@
         <v>93</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G19" t="s">
         <v>55</v>
@@ -1653,12 +1686,12 @@
       <c r="L19" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M19" s="15"/>
+      <c r="M19" s="21"/>
       <c r="N19" s="3">
         <v>9898989899</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1672,7 +1705,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1686,7 +1719,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1700,7 +1733,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1714,7 +1747,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1725,7 +1758,7 @@
         <v>93</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="AD24" t="s">
         <v>25</v>
@@ -1734,19 +1767,19 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F25" s="1"/>
       <c r="AF25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="AG25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1754,7 +1787,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1762,7 +1795,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="15.75">
+    <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -1773,10 +1806,10 @@
         <v>79</v>
       </c>
       <c r="AI28" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -1802,10 +1835,10 @@
       <c r="AB29"/>
       <c r="AC29"/>
       <c r="AI29" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -1831,7 +1864,7 @@
       <c r="AB30"/>
       <c r="AC30"/>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -1857,7 +1890,7 @@
       <c r="AB31"/>
       <c r="AC31"/>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -1877,7 +1910,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -1891,25 +1924,37 @@
         <v>112</v>
       </c>
     </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="W14" r:id="rId2"/>
-    <hyperlink ref="X14" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="C10" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="B32" r:id="rId8"/>
-    <hyperlink ref="C32" r:id="rId9"/>
-    <hyperlink ref="B33" r:id="rId10"/>
-    <hyperlink ref="C33" r:id="rId11"/>
-    <hyperlink ref="F33" r:id="rId12"/>
-    <hyperlink ref="F32" r:id="rId13"/>
-    <hyperlink ref="F13" r:id="rId14"/>
-    <hyperlink ref="B10" r:id="rId15"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="W14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="X14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C5" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B32" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C32" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B33" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C33" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F33" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B8" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F2" r:id="rId19" xr:uid="{2D032192-7392-4F17-86C9-CCF9C2827508}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RevlonUS- Expansion testcases commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlon/RevlonTestData.xlsx
+++ b/src/test/resources/TestData/revlon/RevlonTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBC838C-CBEB-41BC-B5AE-6F292F2BC6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D4FEFB-51D5-4053-B1BD-88E01443D455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="150">
   <si>
     <t>UserName</t>
   </si>
@@ -400,15 +400,27 @@
     <t>Atlanta</t>
   </si>
   <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
     <t>taxrate</t>
   </si>
   <si>
+    <t>Colorado Springs</t>
+  </si>
+  <si>
+    <t>4421 Millburn Dr</t>
+  </si>
+  <si>
     <t>Volume Booster Hair Dryer</t>
   </si>
   <si>
     <t>50$belowproduct</t>
   </si>
   <si>
+    <t>Colorado</t>
+  </si>
+  <si>
     <t>712 Mill Walk NW</t>
   </si>
   <si>
@@ -458,24 +470,6 @@
   </si>
   <si>
     <t>Applygiftcard</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>7.75</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Meriden</t>
-  </si>
-  <si>
-    <t>06450</t>
-  </si>
-  <si>
-    <t>6.35</t>
   </si>
 </sst>
 </file>
@@ -880,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +950,7 @@
         <v>14</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>15</v>
@@ -1016,16 +1010,16 @@
         <v>74</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AH1" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1033,7 +1027,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>92</v>
@@ -1045,7 +1039,7 @@
         <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1065,7 +1059,7 @@
         <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="16.5" x14ac:dyDescent="0.3">
@@ -1081,7 +1075,7 @@
         <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>115</v>
@@ -1123,7 +1117,7 @@
         <v>93</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>106</v>
@@ -1143,8 +1137,8 @@
       <c r="L5" s="15">
         <v>19702</v>
       </c>
-      <c r="M5" s="21" t="s">
-        <v>148</v>
+      <c r="M5" s="21">
+        <v>0</v>
       </c>
       <c r="N5">
         <v>8756941256</v>
@@ -1163,10 +1157,10 @@
         <v>93</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -1178,13 +1172,13 @@
         <v>125</v>
       </c>
       <c r="K6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="L6" s="15">
         <v>30327</v>
       </c>
-      <c r="M6" s="21" t="s">
-        <v>147</v>
+      <c r="M6" s="21">
+        <v>7.75</v>
       </c>
       <c r="N6">
         <v>8756941256</v>
@@ -1203,10 +1197,10 @@
         <v>93</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -1215,16 +1209,16 @@
         <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>151</v>
+        <v>132</v>
+      </c>
+      <c r="L7" s="15">
+        <v>80906</v>
+      </c>
+      <c r="M7" s="21">
+        <v>2.9</v>
       </c>
       <c r="N7">
         <v>8756941256</v>
@@ -1245,7 +1239,7 @@
         <v>93</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G8" t="s">
         <v>103</v>
@@ -1281,7 +1275,7 @@
         <v>93</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G9" t="s">
         <v>104</v>
@@ -1311,10 +1305,10 @@
         <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
         <v>120</v>
@@ -1323,7 +1317,7 @@
         <v>93</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G10" t="s">
         <v>98</v>
@@ -1360,7 +1354,7 @@
         <v>93</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
@@ -1396,7 +1390,7 @@
         <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="I12" t="s">
         <v>31</v>
@@ -1419,7 +1413,7 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" t="s">
@@ -1435,10 +1429,10 @@
       <c r="R13" s="4"/>
       <c r="T13" s="3"/>
       <c r="U13" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AI13" s="8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -1458,7 +1452,7 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="U14" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="V14" t="s">
         <v>22</v>
@@ -1470,7 +1464,7 @@
         <v>24</v>
       </c>
       <c r="AI14" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -1484,7 +1478,7 @@
         <v>93</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G15" t="s">
         <v>30</v>
@@ -1510,7 +1504,7 @@
       </c>
       <c r="O15" s="3"/>
       <c r="U15" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="V15" t="s">
         <v>41</v>
@@ -1531,7 +1525,7 @@
         <v>2020</v>
       </c>
       <c r="AI15" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -1545,7 +1539,7 @@
         <v>93</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G16" t="s">
         <v>30</v>
@@ -1571,7 +1565,7 @@
       </c>
       <c r="O16" s="3"/>
       <c r="U16" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="V16" t="s">
         <v>41</v>
@@ -1592,7 +1586,7 @@
         <v>2020</v>
       </c>
       <c r="AI16" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -1606,7 +1600,7 @@
         <v>93</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G17" t="s">
         <v>55</v>
@@ -1643,7 +1637,7 @@
         <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="U18" t="s">
         <v>50</v>
@@ -1666,7 +1660,7 @@
         <v>93</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G19" t="s">
         <v>55</v>
@@ -1758,7 +1752,7 @@
         <v>93</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AD24" t="s">
         <v>25</v>
@@ -1769,14 +1763,14 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F25" s="1"/>
       <c r="AF25" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="AG25" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -1806,7 +1800,7 @@
         <v>79</v>
       </c>
       <c r="AI28" s="8" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -1835,7 +1829,7 @@
       <c r="AB29"/>
       <c r="AC29"/>
       <c r="AI29" s="8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -1926,10 +1920,10 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="AJ34" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>